<commit_message>
test with chrome, edge
</commit_message>
<xml_diff>
--- a/DATA_EXCEL.xlsx
+++ b/DATA_EXCEL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vinh Hung\source\repos\playwright01\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A37BB24B-D9DD-460A-BA85-4F1F36447259}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{584560EF-D700-4E4C-BD41-6D243AEDF59B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5415" yWindow="3375" windowWidth="17310" windowHeight="9135" xr2:uid="{A3D10778-5BF9-44EB-B3E1-F011D1C9BA2E}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="28">
   <si>
     <t>Page</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>propValue1_6</t>
+  </si>
+  <si>
+    <t>sample.pdf</t>
   </si>
 </sst>
 </file>
@@ -491,7 +494,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,9 +598,8 @@
       <c r="C7" t="s">
         <v>26</v>
       </c>
-      <c r="D7" t="str">
-        <f ca="1">_xlfn.CONCAT("sample_", TEXT(NOW(), "yyyyMMdd\_hhmmss"), ".pdf")</f>
-        <v>sample_20240830_093153.pdf</v>
+      <c r="D7" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>